<commit_message>
removed domin part from sheet name. Made generic for all domains. Any input file should have the below sheet name input files: Requirements Domain Dataelements
</commit_message>
<xml_diff>
--- a/SoftwareDesignUsingNLP/data/Requirements.xlsx
+++ b/SoftwareDesignUsingNLP/data/Requirements.xlsx
@@ -1,20 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="26124"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/swaroopmishra/Desktop/pythonscript/NLP_Project/nWave_softwareDesign/notebook/final/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14180" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="15165" windowHeight="3585" tabRatio="500"/>
   </bookViews>
   <sheets>
-    <sheet name="Banking-Requirements" sheetId="1" r:id="rId1"/>
+    <sheet name="Requirements" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="140000" concurrentCalc="0"/>
+  <calcPr calcId="0" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -634,22 +629,22 @@
   <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C9" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
       <selection pane="bottomRight" activeCell="F12" sqref="F12:G13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.1640625" style="6" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.125" style="6" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="20" style="3" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="47" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="47.1640625" style="3" customWidth="1"/>
+    <col min="4" max="4" width="47.125" style="3" customWidth="1"/>
     <col min="5" max="16384" width="11" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="19" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>9</v>
       </c>
@@ -663,7 +658,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>2</v>
       </c>
@@ -677,7 +672,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>3</v>
       </c>
@@ -691,7 +686,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>4</v>
       </c>
@@ -705,7 +700,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>5</v>
       </c>
@@ -719,7 +714,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>6</v>
       </c>
@@ -733,7 +728,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>7</v>
       </c>
@@ -747,7 +742,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>8</v>
       </c>
@@ -761,7 +756,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="31" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4" ht="30.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>32</v>
       </c>
@@ -775,7 +770,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
         <v>33</v>
       </c>
@@ -789,7 +784,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
         <v>34</v>
       </c>
@@ -803,7 +798,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
         <v>36</v>
       </c>

</xml_diff>